<commit_message>
Trying in OOP - Dict window
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewHorizon\Documents\PythonProjects\EnglishLearn\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBB8D72-592E-4C60-9C0D-2B52CF151CFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B31EBF1-5463-4F80-AB75-0ECE5C8342A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5565" yWindow="3780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="word" sheetId="1" r:id="rId1"/>
-    <sheet name="multiply" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId2"/>
+    <sheet name="multiply" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">word!$A$1:$F$274</definedName>
@@ -33,12 +34,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="202">
   <si>
     <t>птица</t>
   </si>
@@ -578,15 +582,88 @@
   </si>
   <si>
     <t>бутерброд</t>
+  </si>
+  <si>
+    <t>meat</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>biscuits</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>orange juice</t>
+  </si>
+  <si>
+    <t>pasta</t>
+  </si>
+  <si>
+    <t>carrots</t>
+  </si>
+  <si>
+    <t>sausages</t>
+  </si>
+  <si>
+    <t>rice</t>
+  </si>
+  <si>
+    <t>popcorn</t>
+  </si>
+  <si>
+    <t>мясо</t>
+  </si>
+  <si>
+    <t>картошка</t>
+  </si>
+  <si>
+    <t>печенье</t>
+  </si>
+  <si>
+    <t>cookie</t>
+  </si>
+  <si>
+    <t>торт</t>
+  </si>
+  <si>
+    <t>апельсиновый сок</t>
+  </si>
+  <si>
+    <t>макароны</t>
+  </si>
+  <si>
+    <t>морковка</t>
+  </si>
+  <si>
+    <t>сосиски</t>
+  </si>
+  <si>
+    <t>рис</t>
+  </si>
+  <si>
+    <t>попкорн</t>
+  </si>
+  <si>
+    <t>оно</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -601,7 +678,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -609,16 +686,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,9 +1011,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:F274"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F7" sqref="F7:F54"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7:D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1149,10 +1237,12 @@
       <c r="D14" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>201</v>
+      </c>
       <c r="F14" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>it,#это,</v>
+        <v>it,#это,оно</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -2080,7 +2170,7 @@
         <v>day,#день,</v>
       </c>
     </row>
-    <row r="81" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B81" s="2" t="s">
         <v>99</v>
       </c>
@@ -2093,7 +2183,7 @@
         <v>sunny,#солнечно,</v>
       </c>
     </row>
-    <row r="82" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B82" s="2" t="s">
         <v>100</v>
       </c>
@@ -2106,7 +2196,7 @@
         <v>windy,#ветренно,</v>
       </c>
     </row>
-    <row r="83" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="B83" s="2" t="s">
         <v>101</v>
       </c>
@@ -2119,87 +2209,170 @@
         <v>who,#кто,</v>
       </c>
     </row>
-    <row r="84" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D84" s="2"/>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
+        <v>1</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>190</v>
+      </c>
       <c r="E84" s="2"/>
       <c r="F84" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="85" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D85" s="2"/>
+        <v>meat,#мясо,</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85" s="1">
+        <v>1</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>191</v>
+      </c>
       <c r="E85" s="2"/>
       <c r="F85" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="86" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D86" s="2"/>
+        <v>potato,#картошка,</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="1">
+        <v>1</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>192</v>
+      </c>
       <c r="E86" s="2"/>
       <c r="F86" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="87" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D87" s="2"/>
+        <v>biscuits,cookie#печенье,</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="1">
+        <v>1</v>
+      </c>
+      <c r="B87" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>194</v>
+      </c>
       <c r="E87" s="2"/>
       <c r="F87" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="88" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D88" s="2"/>
+        <v>cake,#торт,</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>1</v>
+      </c>
+      <c r="B88" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D88" s="2" t="s">
+        <v>195</v>
+      </c>
       <c r="E88" s="2"/>
       <c r="F88" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="89" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D89" s="2"/>
+        <v>orange juice,#апельсиновый сок,</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
+        <v>1</v>
+      </c>
+      <c r="B89" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="D89" s="2" t="s">
+        <v>196</v>
+      </c>
       <c r="E89" s="2"/>
       <c r="F89" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="90" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D90" s="2"/>
+        <v>pasta,#макароны,</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="1">
+        <v>1</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="D90" s="2" t="s">
+        <v>197</v>
+      </c>
       <c r="E90" s="2"/>
       <c r="F90" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="91" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D91" s="2"/>
+        <v>carrots,#морковка,</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="1">
+        <v>1</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D91" s="2" t="s">
+        <v>198</v>
+      </c>
       <c r="E91" s="2"/>
       <c r="F91" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="92" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D92" s="2"/>
+        <v>sausages,#сосиски,</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>1</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D92" s="2" t="s">
+        <v>199</v>
+      </c>
       <c r="E92" s="2"/>
       <c r="F92" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="93" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
-      <c r="D93" s="2"/>
+        <v>rice,#рис,</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
+        <v>1</v>
+      </c>
+      <c r="B93" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D93" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="E93" s="2"/>
       <c r="F93" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>,#,</v>
-      </c>
-    </row>
-    <row r="94" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+        <v>popcorn,#попкорн,</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
       <c r="F94" s="1" t="str">
@@ -2207,7 +2380,7 @@
         <v>,#,</v>
       </c>
     </row>
-    <row r="95" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
       <c r="F95" s="1" t="str">
@@ -2215,7 +2388,7 @@
         <v>,#,</v>
       </c>
     </row>
-    <row r="96" spans="2:6" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
       <c r="F96" s="1" t="str">
@@ -3374,9 +3547,6 @@
         <filter val="1"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F274">
-      <sortCondition ref="A1:A274"/>
-    </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:C1048576">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
@@ -3386,6 +3556,164 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{008EAE5C-D410-4A58-8D78-08179B67B0AE}">
+  <dimension ref="A1:B23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="4"/>
+    </row>
+    <row r="2" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="3" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B3" s="4"/>
+    </row>
+    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="4"/>
+    </row>
+    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="4"/>
+    </row>
+    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="4"/>
+    </row>
+    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="4"/>
+    </row>
+    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B12" s="4"/>
+    </row>
+    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B13" s="4"/>
+    </row>
+    <row r="14" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="4"/>
+    </row>
+    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B15" s="4"/>
+    </row>
+    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B17" s="4"/>
+    </row>
+    <row r="18" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B21" s="4"/>
+    </row>
+    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B23" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41BEADE2-2796-4F46-8122-A4870913C502}">
   <dimension ref="A1:C33"/>
   <sheetViews>

</xml_diff>